<commit_message>
2023-08-20 update next cosmetic
</commit_message>
<xml_diff>
--- a/public/sheets/dunkbin_next_cosmetic.xlsx
+++ b/public/sheets/dunkbin_next_cosmetic.xlsx
@@ -554,7 +554,7 @@
         <v/>
       </c>
       <c r="G4">
-        <v>822</v>
+        <v>1014</v>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -622,7 +622,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" xml:space="preserve">
+    <row r="6">
       <c r="A6">
         <v>8</v>
       </c>
@@ -632,9 +632,8 @@
       <c r="C6" t="str">
         <v/>
       </c>
-      <c r="D6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Lelouch
-Code Geass</v>
+      <c r="D6" t="str">
+        <v>Sweat Beast</v>
       </c>
       <c r="E6" t="str">
         <v/>
@@ -643,7 +642,7 @@
         <v>Full Head</v>
       </c>
       <c r="G6" t="str">
-        <v/>
+        <v>https://cdn.discordapp.com/attachments/699111007649398865/1132600250603937842/beast_head_2.png</v>
       </c>
       <c r="H6" t="str">
         <v/>
@@ -687,7 +686,7 @@
         <v>Hat</v>
       </c>
       <c r="G7" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1048523933063843931/Dunk_Sweatling_Lelouch_HatHair_V2b_210x210.png</v>
+        <v/>
       </c>
       <c r="H7" t="str">
         <v/>
@@ -775,7 +774,7 @@
         <v>Neck</v>
       </c>
       <c r="G9" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1048523933399404614/Dunk_Sweatling_Lelouch_NeckClothes_V2b_210x210.png</v>
+        <v>https://cdn.discordapp.com/attachments/699111007649398865/1132600250847215656/beast_skin_1.png</v>
       </c>
       <c r="H9" t="str">
         <v/>
@@ -895,13 +894,13 @@
         <v/>
       </c>
       <c r="C12" t="str">
-        <v>omnipotent_0</v>
+        <v>clown_noes666</v>
       </c>
       <c r="D12">
-        <v>42256416</v>
+        <v>469660616</v>
       </c>
       <c r="E12" t="str">
-        <v>260 days</v>
+        <v>115 days</v>
       </c>
       <c r="F12" t="str">
         <v/>
@@ -983,7 +982,7 @@
         <v/>
       </c>
       <c r="C14" t="str">
-        <v>Omnipotent_0</v>
+        <v>clown noes666</v>
       </c>
       <c r="D14" t="str">
         <v/>
@@ -1027,7 +1026,7 @@
         <v/>
       </c>
       <c r="C15" t="str">
-        <v/>
+        <v>Clown_noes666</v>
       </c>
       <c r="D15" t="str">
         <v/>
@@ -1098,7 +1097,7 @@
         <v/>
       </c>
       <c r="L16">
-        <v>822</v>
+        <v>1014</v>
       </c>
       <c r="M16" t="str">
         <v/>

</xml_diff>

<commit_message>
2023-08-23 update next cosmetic
</commit_message>
<xml_diff>
--- a/public/sheets/dunkbin_next_cosmetic.xlsx
+++ b/public/sheets/dunkbin_next_cosmetic.xlsx
@@ -397,41 +397,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>507</v>
+      </c>
+      <c r="B1" t="str">
         <v>row_number</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>col_1</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>Type to search:</v>
       </c>
-      <c r="D1" t="str">
-        <v>col_3</v>
-      </c>
       <c r="E1" t="str">
+        <v>nyakuza mask</v>
+      </c>
+      <c r="F1" t="str">
         <v>col_4</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>col_5</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>col_6</v>
       </c>
-      <c r="H1" t="str">
-        <v>col_7</v>
-      </c>
       <c r="I1" t="str">
-        <v>col_8</v>
+        <v>Nyakuza Mask</v>
       </c>
       <c r="J1" t="str">
-        <v>col_9</v>
+        <v>snekiecr8</v>
       </c>
       <c r="K1" t="str">
         <v>col_10</v>
@@ -442,23 +442,20 @@
       <c r="M1" t="str">
         <v>col_12</v>
       </c>
-      <c r="N1" t="str">
-        <v>col_13</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="B2" t="str">
-        <v/>
-      </c>
       <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
         <v>Here is the oldest cosmetic in the backlog by the least-recently added creator, along with any CITB redeems. Change the selector to see each in turn.</v>
       </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
       <c r="E2" t="str">
         <v/>
       </c>
@@ -486,23 +483,20 @@
       <c r="M2" t="str">
         <v/>
       </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3">
         <v>4</v>
       </c>
-      <c r="B3" t="str">
-        <v/>
-      </c>
       <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
         <v>If there is a red chip in the top right, select the first number in the list to see the current cosmetic  vvvvv</v>
       </c>
-      <c r="D3" t="str">
-        <v/>
-      </c>
       <c r="E3" t="str">
         <v/>
       </c>
@@ -530,35 +524,32 @@
       <c r="M3" t="str">
         <v/>
       </c>
-      <c r="N3" t="str">
-        <v/>
-      </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C4" t="str">
+      <c r="D4" t="str">
         <v>Shop candidates:</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="str">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="str">
         <v>Select row to get info:</v>
       </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4">
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4">
         <v>1014</v>
       </c>
-      <c r="H4" t="str">
-        <v/>
-      </c>
       <c r="I4" t="str">
         <v/>
       </c>
@@ -574,32 +565,29 @@
       <c r="M4" t="str">
         <v/>
       </c>
-      <c r="N4" t="str">
-        <v/>
-      </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5">
         <v>7</v>
       </c>
-      <c r="B5" t="str">
-        <v/>
-      </c>
       <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
         <v>Preview</v>
       </c>
-      <c r="D5" t="str">
+      <c r="E5" t="str">
         <v>Title/notes</v>
       </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
       <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
         <v>Image links</v>
       </c>
-      <c r="G5" t="str">
-        <v/>
-      </c>
       <c r="H5" t="str">
         <v/>
       </c>
@@ -618,35 +606,32 @@
       <c r="M5" t="str">
         <v/>
       </c>
-      <c r="N5" t="str">
-        <v/>
-      </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6">
         <v>8</v>
       </c>
-      <c r="B6" t="str">
-        <v/>
-      </c>
       <c r="C6" t="str">
         <v/>
       </c>
       <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6" t="str">
         <v>Sweat Beast</v>
       </c>
-      <c r="E6" t="str">
-        <v/>
-      </c>
       <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
         <v>Full Head</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <v>https://cdn.discordapp.com/attachments/699111007649398865/1132600250603937842/beast_head_2.png</v>
       </c>
-      <c r="H6" t="str">
-        <v/>
-      </c>
       <c r="I6" t="str">
         <v/>
       </c>
@@ -662,17 +647,14 @@
       <c r="M6" t="str">
         <v/>
       </c>
-      <c r="N6" t="str">
-        <v/>
-      </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7">
         <v>9</v>
       </c>
-      <c r="B7" t="str">
-        <v/>
-      </c>
       <c r="C7" t="str">
         <v/>
       </c>
@@ -683,11 +665,11 @@
         <v/>
       </c>
       <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
         <v>Hat</v>
       </c>
-      <c r="G7" t="str">
-        <v/>
-      </c>
       <c r="H7" t="str">
         <v/>
       </c>
@@ -706,17 +688,14 @@
       <c r="M7" t="str">
         <v/>
       </c>
-      <c r="N7" t="str">
-        <v/>
-      </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8">
         <v>10</v>
       </c>
-      <c r="B8" t="str">
-        <v/>
-      </c>
       <c r="C8" t="str">
         <v/>
       </c>
@@ -727,11 +706,11 @@
         <v/>
       </c>
       <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
         <v>Face</v>
       </c>
-      <c r="G8" t="str">
-        <v/>
-      </c>
       <c r="H8" t="str">
         <v/>
       </c>
@@ -750,17 +729,14 @@
       <c r="M8" t="str">
         <v/>
       </c>
-      <c r="N8" t="str">
-        <v/>
-      </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9">
         <v>11</v>
       </c>
-      <c r="B9" t="str">
-        <v/>
-      </c>
       <c r="C9" t="str">
         <v/>
       </c>
@@ -771,14 +747,14 @@
         <v/>
       </c>
       <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
         <v>Neck</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <v>https://cdn.discordapp.com/attachments/699111007649398865/1132600250847215656/beast_skin_1.png</v>
       </c>
-      <c r="H9" t="str">
-        <v/>
-      </c>
       <c r="I9" t="str">
         <v/>
       </c>
@@ -794,17 +770,14 @@
       <c r="M9" t="str">
         <v/>
       </c>
-      <c r="N9" t="str">
-        <v/>
-      </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+      <c r="B10">
         <v>12</v>
       </c>
-      <c r="B10" t="str">
-        <v/>
-      </c>
       <c r="C10" t="str">
         <v/>
       </c>
@@ -815,11 +788,11 @@
         <v/>
       </c>
       <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
         <v>Body</v>
       </c>
-      <c r="G10" t="str">
-        <v/>
-      </c>
       <c r="H10" t="str">
         <v/>
       </c>
@@ -838,35 +811,32 @@
       <c r="M10" t="str">
         <v/>
       </c>
-      <c r="N10" t="str">
-        <v/>
-      </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11">
         <v>15</v>
       </c>
-      <c r="B11" t="str">
-        <v/>
-      </c>
       <c r="C11" t="str">
+        <v/>
+      </c>
+      <c r="D11" t="str">
         <v>Creator</v>
       </c>
-      <c r="D11" t="str">
+      <c r="E11" t="str">
         <v>Twitch ID</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <v>How long have we been waiting?</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <v>CITB Redeemer(s)</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <v>Redeem Notes</v>
       </c>
-      <c r="H11" t="str">
-        <v/>
-      </c>
       <c r="I11" t="str">
         <v/>
       </c>
@@ -882,29 +852,26 @@
       <c r="M11" t="str">
         <v/>
       </c>
-      <c r="N11" t="str">
-        <v/>
-      </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" t="str">
+        <v/>
+      </c>
+      <c r="B12">
         <v>16</v>
       </c>
-      <c r="B12" t="str">
-        <v/>
-      </c>
       <c r="C12" t="str">
+        <v/>
+      </c>
+      <c r="D12" t="str">
         <v>clown_noes666</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>469660616</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <v>118 days</v>
       </c>
-      <c r="F12" t="str">
-        <v/>
-      </c>
       <c r="G12" t="str">
         <v/>
       </c>
@@ -926,26 +893,23 @@
       <c r="M12" t="str">
         <v/>
       </c>
-      <c r="N12" t="str">
-        <v/>
-      </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" t="str">
+        <v/>
+      </c>
+      <c r="B13">
         <v>18</v>
       </c>
-      <c r="B13" t="str">
-        <v/>
-      </c>
       <c r="C13" t="str">
+        <v/>
+      </c>
+      <c r="D13" t="str">
         <v>Discord alias(es)</v>
       </c>
-      <c r="D13" t="str">
+      <c r="E13" t="str">
         <v>Add aliases and IDs to the UserLookup tab</v>
       </c>
-      <c r="E13" t="str">
-        <v/>
-      </c>
       <c r="F13" t="str">
         <v/>
       </c>
@@ -970,23 +934,20 @@
       <c r="M13" t="str">
         <v/>
       </c>
-      <c r="N13" t="str">
-        <v/>
-      </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" t="str">
+        <v/>
+      </c>
+      <c r="B14">
         <v>19</v>
       </c>
-      <c r="B14" t="str">
-        <v/>
-      </c>
       <c r="C14" t="str">
+        <v/>
+      </c>
+      <c r="D14" t="str">
         <v>clown noes666</v>
       </c>
-      <c r="D14" t="str">
-        <v/>
-      </c>
       <c r="E14" t="str">
         <v/>
       </c>
@@ -1014,23 +975,20 @@
       <c r="M14" t="str">
         <v/>
       </c>
-      <c r="N14" t="str">
-        <v/>
-      </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" t="str">
+        <v/>
+      </c>
+      <c r="B15">
         <v>20</v>
       </c>
-      <c r="B15" t="str">
-        <v/>
-      </c>
       <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
         <v>Clown_noes666</v>
       </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
       <c r="E15" t="str">
         <v/>
       </c>
@@ -1050,25 +1008,22 @@
         <v/>
       </c>
       <c r="K15" t="str">
-        <v/>
+        <v>shop item rows</v>
       </c>
       <c r="L15" t="str">
-        <v>shop item rows</v>
+        <v>citb user(s)</v>
       </c>
       <c r="M15" t="str">
-        <v>citb user(s)</v>
-      </c>
-      <c r="N15" t="str">
         <v>citb comment</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" t="str">
+        <v/>
+      </c>
+      <c r="B16">
         <v>21</v>
       </c>
-      <c r="B16" t="str">
-        <v/>
-      </c>
       <c r="C16" t="str">
         <v/>
       </c>
@@ -1093,22 +1048,61 @@
       <c r="J16" t="str">
         <v/>
       </c>
-      <c r="K16" t="str">
-        <v/>
-      </c>
-      <c r="L16">
+      <c r="K16">
         <v>1014</v>
       </c>
+      <c r="L16" t="str">
+        <v/>
+      </c>
       <c r="M16" t="str">
         <v/>
       </c>
-      <c r="N16" t="str">
-        <v/>
+    </row>
+    <row r="17" xml:space="preserve">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17">
+        <v>22</v>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17">
+        <v>507</v>
+      </c>
+      <c r="L17" t="str" xml:space="preserve">
+        <v xml:space="preserve">Nyakuza Mask
+A hat in time</v>
+      </c>
+      <c r="M17" t="str">
+        <v>snekiecr8</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2023-08-24 update next cosmetic
</commit_message>
<xml_diff>
--- a/public/sheets/dunkbin_next_cosmetic.xlsx
+++ b/public/sheets/dunkbin_next_cosmetic.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -554,7 +554,7 @@
         <v/>
       </c>
       <c r="G4">
-        <v>1027</v>
+        <v>877</v>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -633,8 +633,8 @@
         <v/>
       </c>
       <c r="D6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Count Olaf
-A series of Unfortunate Events</v>
+        <v xml:space="preserve">Meow Face
+Animal Crossing</v>
       </c>
       <c r="E6" t="str">
         <v/>
@@ -643,7 +643,7 @@
         <v>Full Head</v>
       </c>
       <c r="G6" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1104629198011768892/count_olaf_1.png</v>
+        <v/>
       </c>
       <c r="H6" t="str">
         <v/>
@@ -731,7 +731,7 @@
         <v>Face</v>
       </c>
       <c r="G8" t="str">
-        <v/>
+        <v>https://cdn.discordapp.com/attachments/699111007649398865/1062644744498454618/MeowFaceB.png</v>
       </c>
       <c r="H8" t="str">
         <v/>
@@ -775,7 +775,7 @@
         <v>Neck</v>
       </c>
       <c r="G9" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1104629198229884958/count_olaf_jacket_2.png</v>
+        <v/>
       </c>
       <c r="H9" t="str">
         <v/>
@@ -895,13 +895,13 @@
         <v/>
       </c>
       <c r="C12" t="str">
-        <v>clown_noes666</v>
+        <v>darkpulse91</v>
       </c>
       <c r="D12">
-        <v>469660616</v>
+        <v>72148581</v>
       </c>
       <c r="E12" t="str">
-        <v>108 days</v>
+        <v>224 days</v>
       </c>
       <c r="F12" t="str">
         <v/>
@@ -977,13 +977,13 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="str">
         <v/>
       </c>
       <c r="C14" t="str">
-        <v>clown noes666</v>
+        <v/>
       </c>
       <c r="D14" t="str">
         <v/>
@@ -1010,24 +1010,24 @@
         <v/>
       </c>
       <c r="L14" t="str">
-        <v/>
+        <v>shop item rows</v>
       </c>
       <c r="M14" t="str">
-        <v/>
+        <v>citb user(s)</v>
       </c>
       <c r="N14" t="str">
-        <v/>
+        <v>citb comment</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" t="str">
         <v/>
       </c>
       <c r="C15" t="str">
-        <v>Clown_noes666</v>
+        <v/>
       </c>
       <c r="D15" t="str">
         <v/>
@@ -1053,63 +1053,19 @@
       <c r="K15" t="str">
         <v/>
       </c>
-      <c r="L15" t="str">
-        <v>shop item rows</v>
+      <c r="L15">
+        <v>877</v>
       </c>
       <c r="M15" t="str">
-        <v>citb user(s)</v>
+        <v/>
       </c>
       <c r="N15" t="str">
-        <v>citb comment</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>21</v>
-      </c>
-      <c r="B16" t="str">
-        <v/>
-      </c>
-      <c r="C16" t="str">
-        <v/>
-      </c>
-      <c r="D16" t="str">
-        <v/>
-      </c>
-      <c r="E16" t="str">
-        <v/>
-      </c>
-      <c r="F16" t="str">
-        <v/>
-      </c>
-      <c r="G16" t="str">
-        <v/>
-      </c>
-      <c r="H16" t="str">
-        <v/>
-      </c>
-      <c r="I16" t="str">
-        <v/>
-      </c>
-      <c r="J16" t="str">
-        <v/>
-      </c>
-      <c r="K16" t="str">
-        <v/>
-      </c>
-      <c r="L16">
-        <v>1027</v>
-      </c>
-      <c r="M16" t="str">
-        <v/>
-      </c>
-      <c r="N16" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>